<commit_message>
update files dan folder
</commit_message>
<xml_diff>
--- a/Problems/Toileteries/dbase pembelian produk.xlsx
+++ b/Problems/Toileteries/dbase pembelian produk.xlsx
@@ -12,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">tanggal</t>
   </si>
   <si>
+    <t xml:space="preserve">nama_item</t>
+  </si>
+  <si>
     <t xml:space="preserve">satuan</t>
   </si>
   <si>
@@ -26,49 +29,121 @@
     <t xml:space="preserve">jml_masuk</t>
   </si>
   <si>
+    <t xml:space="preserve">penjual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harga_beli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_beli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALKOHOL</t>
+  </si>
+  <si>
     <t xml:space="preserve">LITER</t>
   </si>
   <si>
     <t xml:space="preserve">CSYHO008</t>
   </si>
   <si>
+    <t xml:space="preserve">Stock Larutan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAND SANITIZER</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSYHO009</t>
   </si>
   <si>
+    <t xml:space="preserve">Mitra Jaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">297000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HANDSOAP</t>
+  </si>
+  <si>
     <t xml:space="preserve">GALON</t>
   </si>
   <si>
     <t xml:space="preserve">CSYHO004</t>
   </si>
   <si>
+    <t xml:space="preserve">117000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">270000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAMPER</t>
+  </si>
+  <si>
     <t xml:space="preserve">PACK</t>
   </si>
   <si>
     <t xml:space="preserve">CSYHO003</t>
   </si>
   <si>
+    <t xml:space="preserve">23000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEBEK BIRU</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSYHO002</t>
   </si>
   <si>
+    <t xml:space="preserve">15858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TISSUE TOILET</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROLL</t>
   </si>
   <si>
     <t xml:space="preserve">CSYHO001</t>
   </si>
   <si>
+    <t xml:space="preserve">1361.73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOTOL POMPA 500 ML</t>
+  </si>
+  <si>
     <t xml:space="preserve">PCS</t>
   </si>
   <si>
     <t xml:space="preserve">CSYHO010</t>
   </si>
   <si>
+    <t xml:space="preserve">Mayoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PENGHARUM RUANGAN (STELLA)</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOTOL</t>
   </si>
   <si>
     <t xml:space="preserve">CSYHO007</t>
   </si>
   <si>
+    <t xml:space="preserve">ANTI NYAMUK SEMPROT (BAYGON/HIT)</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSYHO006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAKAN IKAN</t>
   </si>
   <si>
     <t xml:space="preserve">CSYHO005</t>
@@ -424,19 +499,43 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44223</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="n">
         <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -444,13 +543,25 @@
         <v>44224</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="n">
         <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="n">
+        <v>14850000</v>
       </c>
     </row>
     <row r="4">
@@ -458,13 +569,25 @@
         <v>44256</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="n">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="n">
         <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1170000</v>
       </c>
     </row>
     <row r="5">
@@ -472,13 +595,25 @@
         <v>44274</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
         <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -486,13 +621,25 @@
         <v>44274</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="n">
         <v>100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="n">
+        <v>27000000</v>
       </c>
     </row>
     <row r="7">
@@ -500,13 +647,25 @@
         <v>44277</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="n">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="n">
         <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="n">
+        <v>690000</v>
       </c>
     </row>
     <row r="8">
@@ -514,13 +673,25 @@
         <v>44286</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="n">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="n">
         <v>60</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="n">
+        <v>951480</v>
       </c>
     </row>
     <row r="9">
@@ -528,13 +699,25 @@
         <v>44323</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="n">
         <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -542,13 +725,25 @@
         <v>44336</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="n">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="n">
         <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="n">
+        <v>690000</v>
       </c>
     </row>
     <row r="11">
@@ -556,13 +751,25 @@
         <v>44336</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="n">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="n">
         <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1170000</v>
       </c>
     </row>
     <row r="12">
@@ -570,13 +777,25 @@
         <v>44340</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="n">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="n">
         <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="n">
+        <v>570888</v>
       </c>
     </row>
     <row r="13">
@@ -584,13 +803,25 @@
         <v>44344</v>
       </c>
       <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1000</v>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1361730</v>
       </c>
     </row>
     <row r="14">
@@ -598,13 +829,25 @@
         <v>44356</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="n">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="n">
         <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -612,13 +855,25 @@
         <v>44249</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="n">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="n">
         <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="n">
+        <v>200000</v>
       </c>
     </row>
     <row r="16">
@@ -626,13 +881,25 @@
         <v>44364</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="n">
         <v>100</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" t="n">
+        <v>27000000</v>
       </c>
     </row>
     <row r="17">
@@ -640,13 +907,25 @@
         <v>44383</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="n">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="n">
         <v>100</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" t="n">
+        <v>27000000</v>
       </c>
     </row>
     <row r="18">
@@ -654,13 +933,25 @@
         <v>44386</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="n">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="n">
         <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1170000</v>
       </c>
     </row>
     <row r="19">
@@ -668,13 +959,25 @@
         <v>44386</v>
       </c>
       <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F19" t="s">
         <v>12</v>
       </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" t="n">
-        <v>2000</v>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2723460</v>
       </c>
     </row>
     <row r="20">
@@ -682,13 +985,25 @@
         <v>44389</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="n">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="n">
         <v>50</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1150000</v>
       </c>
     </row>
     <row r="21">
@@ -696,13 +1011,25 @@
         <v>44390</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="n">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
         <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -710,13 +1037,25 @@
         <v>44406</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" t="n">
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="n">
         <v>60</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" t="n">
+        <v>951480</v>
       </c>
     </row>
     <row r="23">
@@ -724,13 +1063,25 @@
         <v>44431</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="n">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
         <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -738,13 +1089,21 @@
         <v>44460</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" t="n">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="n">
         <v>60</v>
+      </c>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -752,13 +1111,21 @@
         <v>44454</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="n">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="n">
         <v>40</v>
+      </c>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -766,13 +1133,21 @@
         <v>44454</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="n">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="n">
         <v>10</v>
+      </c>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -780,13 +1155,21 @@
         <v>44487</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" t="n">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="n">
         <v>30</v>
+      </c>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -794,13 +1177,21 @@
         <v>44506</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" t="n">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" t="n">
         <v>1500</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -808,13 +1199,21 @@
         <v>44506</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" t="n">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" t="n">
         <v>34</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -822,13 +1221,21 @@
         <v>44506</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="n">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="n">
         <v>10</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -836,13 +1243,21 @@
         <v>44532</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="n">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="n">
         <v>10</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -850,13 +1265,21 @@
         <v>44532</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" t="n">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="n">
         <v>40</v>
+      </c>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -864,13 +1287,21 @@
         <v>44540</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" t="n">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" t="n">
         <v>2000</v>
+      </c>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -878,13 +1309,21 @@
         <v>45274</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" t="n">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" t="n">
         <v>2300</v>
+      </c>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -892,13 +1331,21 @@
         <v>44566</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" t="n">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" t="n">
         <v>2000</v>
+      </c>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -906,13 +1353,21 @@
         <v>44694</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" t="n">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" t="n">
         <v>2000</v>
+      </c>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -920,13 +1375,21 @@
         <v>44845</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" t="n">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="n">
         <v>2000</v>
+      </c>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -934,13 +1397,21 @@
         <v>44887</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" t="n">
+        <v>30</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" t="n">
         <v>2000</v>
+      </c>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -948,13 +1419,21 @@
         <v>44758</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" t="n">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" t="n">
         <v>1900</v>
+      </c>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -962,13 +1441,21 @@
         <v>44802</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" t="n">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" t="n">
         <v>1600</v>
+      </c>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -976,13 +1463,21 @@
         <v>45173</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" t="n">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" t="n">
         <v>1000</v>
+      </c>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -990,13 +1485,21 @@
         <v>45196</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" t="n">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" t="n">
         <v>1000</v>
+      </c>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1004,13 +1507,21 @@
         <v>45210</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" t="n">
+        <v>30</v>
+      </c>
+      <c r="D43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" t="n">
         <v>1000</v>
+      </c>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1018,13 +1529,21 @@
         <v>45229</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" t="n">
+        <v>30</v>
+      </c>
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" t="n">
         <v>1000</v>
+      </c>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1032,13 +1551,21 @@
         <v>45252</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" t="n">
+        <v>30</v>
+      </c>
+      <c r="D45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" t="n">
         <v>900</v>
+      </c>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1046,13 +1573,21 @@
         <v>45168</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" t="n">
+        <v>30</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" t="n">
         <v>386</v>
+      </c>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1060,13 +1595,21 @@
         <v>45275</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" t="n">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" t="n">
         <v>240</v>
+      </c>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1074,13 +1617,21 @@
         <v>44839</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" t="n">
+        <v>30</v>
+      </c>
+      <c r="D48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" t="n">
         <v>200</v>
+      </c>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1088,27 +1639,41 @@
         <v>44628</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" t="n">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="n">
         <v>124</v>
       </c>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>45230</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" t="n">
+        <v>23</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="n">
         <v>120</v>
+      </c>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1116,13 +1681,21 @@
         <v>44691</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" t="n">
+        <v>30</v>
+      </c>
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" t="n">
         <v>100</v>
+      </c>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1130,13 +1703,21 @@
         <v>45250</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" t="n">
+        <v>30</v>
+      </c>
+      <c r="D52" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" t="n">
         <v>100</v>
+      </c>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1144,13 +1725,21 @@
         <v>45272</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" t="n">
+        <v>30</v>
+      </c>
+      <c r="D53" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" t="n">
         <v>100</v>
+      </c>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1158,13 +1747,21 @@
         <v>45274</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" t="n">
+        <v>30</v>
+      </c>
+      <c r="D54" t="s">
+        <v>31</v>
+      </c>
+      <c r="E54" t="n">
         <v>100</v>
+      </c>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1172,13 +1769,21 @@
         <v>44567</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" t="n">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" t="n">
         <v>95</v>
+      </c>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1186,13 +1791,21 @@
         <v>45168</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" t="n">
+        <v>23</v>
+      </c>
+      <c r="D56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" t="n">
         <v>88</v>
+      </c>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1200,13 +1813,21 @@
         <v>44827</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" t="n">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" t="n">
         <v>80</v>
+      </c>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1214,13 +1835,21 @@
         <v>45168</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" t="n">
+        <v>23</v>
+      </c>
+      <c r="D58" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" t="n">
         <v>71</v>
+      </c>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1228,13 +1857,21 @@
         <v>44706</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" t="n">
+        <v>23</v>
+      </c>
+      <c r="D59" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" t="n">
         <v>60</v>
+      </c>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1242,13 +1879,21 @@
         <v>44756</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" t="n">
+        <v>23</v>
+      </c>
+      <c r="D60" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" t="n">
         <v>60</v>
+      </c>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1256,13 +1901,21 @@
         <v>45208</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C61" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" t="n">
+        <v>23</v>
+      </c>
+      <c r="D61" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" t="n">
         <v>60</v>
+      </c>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1270,13 +1923,21 @@
         <v>44659</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="n">
+        <v>23</v>
+      </c>
+      <c r="D62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" t="n">
         <v>50</v>
+      </c>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1284,13 +1945,21 @@
         <v>44823</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="n">
+        <v>23</v>
+      </c>
+      <c r="D63" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" t="n">
         <v>50</v>
+      </c>
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1298,13 +1967,21 @@
         <v>44840</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
-      </c>
-      <c r="D64" t="n">
+        <v>23</v>
+      </c>
+      <c r="D64" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" t="n">
         <v>50</v>
+      </c>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1312,13 +1989,21 @@
         <v>45202</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>10</v>
-      </c>
-      <c r="D65" t="n">
+        <v>23</v>
+      </c>
+      <c r="D65" t="s">
+        <v>24</v>
+      </c>
+      <c r="E65" t="n">
         <v>50</v>
+      </c>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1326,13 +2011,21 @@
         <v>45250</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
-      </c>
-      <c r="D66" t="n">
+        <v>23</v>
+      </c>
+      <c r="D66" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" t="n">
         <v>50</v>
+      </c>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1340,13 +2033,21 @@
         <v>44851</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
-      </c>
-      <c r="D67" t="n">
+        <v>23</v>
+      </c>
+      <c r="D67" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67" t="n">
         <v>48</v>
+      </c>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1354,13 +2055,21 @@
         <v>44908</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" t="n">
+        <v>23</v>
+      </c>
+      <c r="D68" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" t="n">
         <v>48</v>
+      </c>
+      <c r="F68"/>
+      <c r="G68"/>
+      <c r="H68" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1368,27 +2077,41 @@
         <v>44628</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" t="n">
+        <v>9</v>
+      </c>
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" t="n">
         <v>45</v>
       </c>
+      <c r="F69"/>
+      <c r="G69"/>
+      <c r="H69"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
         <v>44564</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C70" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" t="n">
+        <v>23</v>
+      </c>
+      <c r="D70" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" t="n">
         <v>40</v>
+      </c>
+      <c r="F70"/>
+      <c r="G70"/>
+      <c r="H70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1396,13 +2119,21 @@
         <v>44691</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C71" t="s">
-        <v>10</v>
-      </c>
-      <c r="D71" t="n">
+        <v>23</v>
+      </c>
+      <c r="D71" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" t="n">
         <v>40</v>
+      </c>
+      <c r="F71"/>
+      <c r="G71"/>
+      <c r="H71" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1410,13 +2141,21 @@
         <v>44753</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" t="n">
+        <v>23</v>
+      </c>
+      <c r="D72" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" t="n">
         <v>40</v>
+      </c>
+      <c r="F72"/>
+      <c r="G72"/>
+      <c r="H72" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1424,13 +2163,21 @@
         <v>44782</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" t="n">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" t="n">
         <v>35</v>
+      </c>
+      <c r="F73"/>
+      <c r="G73"/>
+      <c r="H73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1438,13 +2185,21 @@
         <v>44706</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" t="n">
+        <v>9</v>
+      </c>
+      <c r="D74" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" t="n">
         <v>30</v>
+      </c>
+      <c r="F74"/>
+      <c r="G74"/>
+      <c r="H74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1452,13 +2207,21 @@
         <v>44901</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" t="n">
+        <v>9</v>
+      </c>
+      <c r="D75" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75" t="n">
         <v>25</v>
+      </c>
+      <c r="F75"/>
+      <c r="G75"/>
+      <c r="H75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1466,13 +2229,21 @@
         <v>45275</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" t="n">
+        <v>18</v>
+      </c>
+      <c r="D76" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" t="n">
         <v>15</v>
+      </c>
+      <c r="F76"/>
+      <c r="G76"/>
+      <c r="H76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1480,13 +2251,21 @@
         <v>44567</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" t="n">
+        <v>18</v>
+      </c>
+      <c r="D77" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" t="n">
         <v>10</v>
+      </c>
+      <c r="F77"/>
+      <c r="G77"/>
+      <c r="H77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1494,13 +2273,21 @@
         <v>45188</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C78" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" t="n">
+        <v>18</v>
+      </c>
+      <c r="D78" t="s">
+        <v>19</v>
+      </c>
+      <c r="E78" t="n">
         <v>10</v>
+      </c>
+      <c r="F78"/>
+      <c r="G78"/>
+      <c r="H78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -1508,13 +2295,21 @@
         <v>45244</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" t="n">
+        <v>18</v>
+      </c>
+      <c r="D79" t="s">
+        <v>19</v>
+      </c>
+      <c r="E79" t="n">
         <v>10</v>
+      </c>
+      <c r="F79"/>
+      <c r="G79"/>
+      <c r="H79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -1522,27 +2317,41 @@
         <v>44628</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" t="n">
+        <v>34</v>
+      </c>
+      <c r="D80" t="s">
+        <v>35</v>
+      </c>
+      <c r="E80" t="n">
         <v>6</v>
       </c>
+      <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
         <v>44572</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" t="n">
+        <v>9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81" t="n">
         <v>5</v>
+      </c>
+      <c r="F81"/>
+      <c r="G81"/>
+      <c r="H81" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1550,13 +2359,21 @@
         <v>44739</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C82" t="s">
-        <v>8</v>
-      </c>
-      <c r="D82" t="n">
+        <v>18</v>
+      </c>
+      <c r="D82" t="s">
+        <v>19</v>
+      </c>
+      <c r="E82" t="n">
         <v>5</v>
+      </c>
+      <c r="F82"/>
+      <c r="G82"/>
+      <c r="H82" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -1564,13 +2381,21 @@
         <v>44770</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" t="n">
+        <v>18</v>
+      </c>
+      <c r="D83" t="s">
+        <v>19</v>
+      </c>
+      <c r="E83" t="n">
         <v>5</v>
+      </c>
+      <c r="F83"/>
+      <c r="G83"/>
+      <c r="H83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -1578,13 +2403,21 @@
         <v>44810</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" t="n">
+        <v>18</v>
+      </c>
+      <c r="D84" t="s">
+        <v>19</v>
+      </c>
+      <c r="E84" t="n">
         <v>5</v>
+      </c>
+      <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -1592,13 +2425,21 @@
         <v>44827</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" t="n">
+        <v>18</v>
+      </c>
+      <c r="D85" t="s">
+        <v>19</v>
+      </c>
+      <c r="E85" t="n">
         <v>5</v>
+      </c>
+      <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -1606,13 +2447,21 @@
         <v>44869</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>8</v>
-      </c>
-      <c r="D86" t="n">
+        <v>18</v>
+      </c>
+      <c r="D86" t="s">
+        <v>19</v>
+      </c>
+      <c r="E86" t="n">
         <v>5</v>
+      </c>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1620,13 +2469,21 @@
         <v>44902</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C87" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" t="n">
+        <v>18</v>
+      </c>
+      <c r="D87" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87" t="n">
         <v>5</v>
+      </c>
+      <c r="F87"/>
+      <c r="G87"/>
+      <c r="H87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -1634,13 +2491,21 @@
         <v>45168</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>8</v>
-      </c>
-      <c r="D88" t="n">
+        <v>18</v>
+      </c>
+      <c r="D88" t="s">
+        <v>19</v>
+      </c>
+      <c r="E88" t="n">
         <v>5</v>
+      </c>
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1648,13 +2513,21 @@
         <v>44701</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C89" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" t="n">
+        <v>18</v>
+      </c>
+      <c r="D89" t="s">
+        <v>19</v>
+      </c>
+      <c r="E89" t="n">
         <v>4</v>
+      </c>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -1662,13 +2535,21 @@
         <v>44840</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" t="n">
+        <v>18</v>
+      </c>
+      <c r="D90" t="s">
+        <v>19</v>
+      </c>
+      <c r="E90" t="n">
         <v>4</v>
+      </c>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -1676,13 +2557,21 @@
         <v>44796</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D91" t="n">
+        <v>18</v>
+      </c>
+      <c r="D91" t="s">
+        <v>19</v>
+      </c>
+      <c r="E91" t="n">
         <v>3</v>
+      </c>
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -1690,13 +2579,21 @@
         <v>45272</v>
       </c>
       <c r="B92" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C92" t="s">
-        <v>17</v>
-      </c>
-      <c r="D92" t="n">
+        <v>39</v>
+      </c>
+      <c r="D92" t="s">
+        <v>40</v>
+      </c>
+      <c r="E92" t="n">
         <v>3</v>
+      </c>
+      <c r="F92"/>
+      <c r="G92"/>
+      <c r="H92" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -1704,55 +2601,81 @@
         <v>44628</v>
       </c>
       <c r="B93" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C93" t="s">
-        <v>17</v>
-      </c>
-      <c r="D93" t="n">
+        <v>39</v>
+      </c>
+      <c r="D93" t="s">
+        <v>40</v>
+      </c>
+      <c r="E93" t="n">
         <v>2</v>
       </c>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
         <v>44645</v>
       </c>
       <c r="B94" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D94" t="n">
+        <v>39</v>
+      </c>
+      <c r="D94" t="s">
+        <v>40</v>
+      </c>
+      <c r="E94" t="n">
         <v>2</v>
       </c>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
         <v>44645</v>
       </c>
       <c r="B95" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C95" t="s">
-        <v>18</v>
-      </c>
-      <c r="D95" t="n">
+        <v>39</v>
+      </c>
+      <c r="D95" t="s">
+        <v>42</v>
+      </c>
+      <c r="E95" t="n">
         <v>2</v>
       </c>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
         <v>45168</v>
       </c>
       <c r="B96" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C96" t="s">
-        <v>19</v>
-      </c>
-      <c r="D96" t="n">
+        <v>23</v>
+      </c>
+      <c r="D96" t="s">
+        <v>44</v>
+      </c>
+      <c r="E96" t="n">
         <v>2</v>
+      </c>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -1760,13 +2683,21 @@
         <v>45259</v>
       </c>
       <c r="B97" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C97" t="s">
-        <v>19</v>
-      </c>
-      <c r="D97" t="n">
+        <v>23</v>
+      </c>
+      <c r="D97" t="s">
+        <v>44</v>
+      </c>
+      <c r="E97" t="n">
         <v>2</v>
+      </c>
+      <c r="F97"/>
+      <c r="G97"/>
+      <c r="H97" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -1774,13 +2705,21 @@
         <v>45263</v>
       </c>
       <c r="B98" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C98" t="s">
-        <v>19</v>
-      </c>
-      <c r="D98" t="n">
+        <v>23</v>
+      </c>
+      <c r="D98" t="s">
+        <v>44</v>
+      </c>
+      <c r="E98" t="n">
         <v>2</v>
+      </c>
+      <c r="F98"/>
+      <c r="G98"/>
+      <c r="H98" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -1788,13 +2727,21 @@
         <v>45272</v>
       </c>
       <c r="B99" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C99" t="s">
-        <v>18</v>
-      </c>
-      <c r="D99" t="n">
+        <v>39</v>
+      </c>
+      <c r="D99" t="s">
+        <v>42</v>
+      </c>
+      <c r="E99" t="n">
         <v>2</v>
+      </c>
+      <c r="F99"/>
+      <c r="G99"/>
+      <c r="H99" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -1802,13 +2749,21 @@
         <v>44840</v>
       </c>
       <c r="B100" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C100" t="s">
-        <v>8</v>
-      </c>
-      <c r="D100" t="n">
+        <v>18</v>
+      </c>
+      <c r="D100" t="s">
+        <v>19</v>
+      </c>
+      <c r="E100" t="n">
         <v>1</v>
+      </c>
+      <c r="F100"/>
+      <c r="G100"/>
+      <c r="H100" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -1816,13 +2771,21 @@
         <v>45168</v>
       </c>
       <c r="B101" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C101" t="s">
-        <v>18</v>
-      </c>
-      <c r="D101" t="n">
+        <v>39</v>
+      </c>
+      <c r="D101" t="s">
+        <v>42</v>
+      </c>
+      <c r="E101" t="n">
         <v>1</v>
+      </c>
+      <c r="F101"/>
+      <c r="G101"/>
+      <c r="H101" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>